<commit_message>
Bug fixes, formatting in excels
</commit_message>
<xml_diff>
--- a/testovani/tvorba_formulare.xlsx
+++ b/testovani/tvorba_formulare.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrych/Desktop/DiplomaTheses/testovani/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F419B98-DE45-9B48-942C-85157D782D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388C9A09-B800-CE42-AAFF-BD3C36C60024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Odpovědi formuláře 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tvorba formuláře" sheetId="1" r:id="rId1"/>
+    <sheet name="Grafy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -154,7 +155,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -389,6 +389,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -403,22 +404,759 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>115340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Graf odpovědí Formulářů. Název otázky: Rád/a bych aplikaci používal/a opakovaně. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53684078-CA2E-F7A6-FDE8-C8095716C657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="0"/>
+          <a:ext cx="7188199" cy="3417340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>594711</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Graf odpovědí Formulářů. Název otázky: Aplikace je zbytečně složitá&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DA5EF61-BC3F-3817-0475-2E258D13127F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12701" y="3416300"/>
+          <a:ext cx="7186010" cy="3416300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>621425</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Graf odpovědí Formulářů. Název otázky: Aplikace se snadno používá&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A87D98F5-F7B9-B782-EF80-8048C1AE04CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12701" y="6807201"/>
+          <a:ext cx="7212724" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>31854</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Graf odpovědí Formulářů. Název otázky: Potřeboval bych pomoc člověka z technické podpory, abych mohl/a aplikaci používat&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{625BB5E5-3133-EFD2-E583-986C007F71E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="10134601"/>
+          <a:ext cx="7226300" cy="3435453"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635001</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>152192</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Graf odpovědí Formulářů. Název otázky: Různé funkce aplikace jsou do ní dobře začleněny. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF453D45-8F5E-D5FE-9B16-2CF84779DB81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="13550900"/>
+          <a:ext cx="7239000" cy="3441492"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635439</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Graf odpovědí Formulářů. Název otázky: Aplikace je příliš nekonzistentní&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA68A7E0-C007-BA36-29DC-889E0C5DE1A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="16891000"/>
+          <a:ext cx="7239438" cy="3441700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>126791</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Graf odpovědí Formulářů. Název otázky: Řekl/a bych, že většina lidí se s aplikací naučí pracovat rychle&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3221B624-F701-2AD6-7C73-203A7C5D82D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="20294600"/>
+          <a:ext cx="7239000" cy="3441491"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>126166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Graf odpovědí Formulářů. Název otázky: Aplikace je příliš neohrabaná&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45FDD545-8691-90DA-B23F-5F406CBF5FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="23583899"/>
+          <a:ext cx="7264400" cy="3453567"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>547</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>627</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Graf odpovědí Formulářů. Název otázky: Při práci s aplikací se cítím jistě&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5849054C-22AF-8096-CE3A-EE3F897E885F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="90309700"/>
+          <a:ext cx="27889200" cy="13258800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>630</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>710</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Graf odpovědí Formulářů. Název otázky: Musel/a jsem se hodně naučit, než jsem s aplikací dokázal/a pracovat&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37555985-3F18-D208-ACF3-768C9259F29D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="104013000"/>
+          <a:ext cx="27889200" cy="13258800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>688865</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="Graf odpovědí Formulářů. Název otázky: Při práci s aplikací se cítím jistě&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E048BA3B-D8CF-2B8A-2EDC-E00C17D73CF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="26898600"/>
+          <a:ext cx="7292865" cy="3467100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>688863</xdr:colOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Graf odpovědí Formulářů. Název otázky: Musel/a jsem se hodně naučit, než jsem s aplikací dokázal/a pracovat&#10;. Počet odpovědí: 5 odpovědí.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E45F1E-C318-4847-F3E8-DFF296CB7BB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="30251401"/>
+          <a:ext cx="7292863" cy="3467099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{066E6FFA-76E0-DB49-94DD-5ACF42F77CEF}" name="Table3" displayName="Table3" ref="A1:L7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{066E6FFA-76E0-DB49-94DD-5ACF42F77CEF}" name="Table3" displayName="Table3" ref="A1:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L7" xr:uid="{066E6FFA-76E0-DB49-94DD-5ACF42F77CEF}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{10022671-BBF0-F447-A1FA-C9A425288D35}" name=" " dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{2E074DA6-0608-594B-B4BF-04541976B382}" name="Rád/a bych aplikaci používal/a opakovaně" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A24F43FA-BC2D-204E-BE69-925BE6977B9A}" name="Aplikace je zbytečně složitá" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7BE42511-26A0-F54C-AB29-AE83BB73E348}" name="Aplikace se snadno používá" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{0D2BA80E-0F6F-C141-8DAD-CE5F098C14EE}" name="Potřeboval bych pomoc člověka z technické podpory, abych mohl/a aplikaci používat" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{4ED96164-D3F1-794B-AC12-7D04CCC5C54E}" name="Různé funkce aplikace jsou do ní dobře začleněny" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E48CC4CD-93E0-554F-A6DC-4BFA871D0DC3}" name="Aplikace je příliš nekonzistentní" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{2A6C7A09-20C0-E44D-B400-830F42609FCE}" name="Řekl/a bych, že většina lidí se s aplikací naučí pracovat rychle" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{7FFB883D-BF45-304C-816F-F0FC0C179172}" name="Aplikace je příliš neohrabaná" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5C1A9E85-F92A-AB41-9774-CAAD56E60349}" name="Při práci s aplikací se cítím jistě" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{7E96571D-C38F-6C45-AD8F-D618DF1C40F8}" name="Musel/a jsem se hodně naučit, než jsem s aplikací dokázal/a pracovat" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C4CA6185-9B3D-8D4A-852A-006B2BD52265}" name="SUS skóre" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{10022671-BBF0-F447-A1FA-C9A425288D35}" name=" " dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{2E074DA6-0608-594B-B4BF-04541976B382}" name="Rád/a bych aplikaci používal/a opakovaně" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A24F43FA-BC2D-204E-BE69-925BE6977B9A}" name="Aplikace je zbytečně složitá" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{7BE42511-26A0-F54C-AB29-AE83BB73E348}" name="Aplikace se snadno používá" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{0D2BA80E-0F6F-C141-8DAD-CE5F098C14EE}" name="Potřeboval bych pomoc člověka z technické podpory, abych mohl/a aplikaci používat" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{4ED96164-D3F1-794B-AC12-7D04CCC5C54E}" name="Různé funkce aplikace jsou do ní dobře začleněny" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E48CC4CD-93E0-554F-A6DC-4BFA871D0DC3}" name="Aplikace je příliš nekonzistentní" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{2A6C7A09-20C0-E44D-B400-830F42609FCE}" name="Řekl/a bych, že většina lidí se s aplikací naučí pracovat rychle" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{7FFB883D-BF45-304C-816F-F0FC0C179172}" name="Aplikace je příliš neohrabaná" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{5C1A9E85-F92A-AB41-9774-CAAD56E60349}" name="Při práci s aplikací se cítím jistě" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{7E96571D-C38F-6C45-AD8F-D618DF1C40F8}" name="Musel/a jsem se hodně naučit, než jsem s aplikací dokázal/a pracovat" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{C4CA6185-9B3D-8D4A-852A-006B2BD52265}" name="SUS skóre" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,7 +1366,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -889,6 +1627,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F39E61-68CC-224C-867D-0DB223E18335}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{2beeedd2-97cd-4871-8d96-80d2b8fe033c}" enabled="1" method="Standard" siteId="{67266d43-8de7-494d-9ed8-3d1bd3b3a764}" contentBits="0" removed="0"/>

</xml_diff>